<commit_message>
The chromedriver file has been updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestDataForApachePoi.xlsx
+++ b/src/test/resources/testdata/TestDataForApachePoi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janal\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janal\OneDrive\Desktop\TEK School\Projects\MyProjects\bddautomationframework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610B58F4-7C52-4373-BAF1-6E79A8EDC076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D730E3-3E39-443E-ACAD-1609961100F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{401F2730-8C87-4A62-A8C1-25401F63E7F8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>first_name</t>
   </si>
@@ -75,6 +75,15 @@
   </si>
   <si>
     <t>abcd</t>
+  </si>
+  <si>
+    <t>Anisa</t>
+  </si>
+  <si>
+    <t>anisa@gmail.com</t>
+  </si>
+  <si>
+    <t>xyz123</t>
   </si>
 </sst>
 </file>
@@ -494,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81FEE414-B182-42E8-A1B0-0D7506CB558D}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -569,12 +578,33 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>2023439873</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{55230725-B960-4054-8127-872CA085833A}"/>
     <hyperlink ref="C3" r:id="rId2" xr:uid="{5F48B6B0-EEC9-44E5-89FB-4F34B7E0342B}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{879C0DD8-3904-46A5-A874-5B61BD8A8339}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
The project is restored back to default
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/TestDataForApachePoi.xlsx
+++ b/src/test/resources/testdata/TestDataForApachePoi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janal\OneDrive\Desktop\TEK School\Projects\MyProjects\bddautomationframework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D730E3-3E39-443E-ACAD-1609961100F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B885E0E-2EEE-4B2E-9A36-CEE4945C52A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{401F2730-8C87-4A62-A8C1-25401F63E7F8}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{401F2730-8C87-4A62-A8C1-25401F63E7F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,28 +62,28 @@
     <t>Faizi</t>
   </si>
   <si>
-    <t>janfaizi@gmail.com</t>
-  </si>
-  <si>
     <t>janF</t>
   </si>
   <si>
     <t>Ali</t>
   </si>
   <si>
-    <t>alijan@tek.com</t>
-  </si>
-  <si>
     <t>abcd</t>
   </si>
   <si>
     <t>Anisa</t>
   </si>
   <si>
-    <t>anisa@gmail.com</t>
-  </si>
-  <si>
     <t>xyz123</t>
+  </si>
+  <si>
+    <t>janfaizi1@gmail.com</t>
+  </si>
+  <si>
+    <t>alijan2@tek.com</t>
+  </si>
+  <si>
+    <t>anisa2@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,56 +546,56 @@
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1">
         <v>2027904312</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>2023458793</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4">
         <v>2023439873</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>